<commit_message>
modify to be monthly and yearly and only 1 scenario
</commit_message>
<xml_diff>
--- a/revenue-streamlit/tenancy_list_scenario_01C.xlsx
+++ b/revenue-streamlit/tenancy_list_scenario_01C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8db03e8e420626a2/Office/AMG/Development/office/revenue-streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{1E26A472-73F2-904F-A311-C7087A595554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC999BFA-E9AC-574B-A147-149A7CCDFFA7}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{1E26A472-73F2-904F-A311-C7087A595554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73B120C8-34EF-CF48-AF9F-5DF35ACC4A6A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="33260" windowHeight="21160" tabRatio="765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21500" tabRatio="765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -1691,19 +1691,19 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2538,7 +2538,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>288616</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>77683</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2610,13 +2610,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>234894</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>86989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>276703</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>32053</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2688,13 +2688,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>222981</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>131271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>264790</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>157345</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2765,6 +2765,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Product_Type" xr10:uid="{0FBB730F-8D21-DE4E-82F5-FD01F9F099FA}" sourceName="Product_Type">
   <extLst>
@@ -2809,11 +2813,6 @@
     <filterColumn colId="4">
       <filters>
         <filter val="Office"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Y"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3140,7 +3139,7 @@
   <dimension ref="B4:J7"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3155,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>44562</v>
+        <v>44927</v>
       </c>
       <c r="I4" t="s">
         <v>133</v>
@@ -3166,7 +3165,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>48579</v>
+        <v>48944</v>
       </c>
       <c r="I5" t="s">
         <v>131</v>
@@ -3215,8 +3214,8 @@
   <dimension ref="A1:N158"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3791,7 +3790,7 @@
       </c>
       <c r="N13" s="20"/>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -3918,7 +3917,7 @@
       </c>
       <c r="N16" s="20"/>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="29">
         <v>16</v>
       </c>
@@ -4006,7 +4005,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="29">
         <v>18</v>
       </c>
@@ -4050,7 +4049,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="29">
         <v>18</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <v>19</v>
       </c>
@@ -4130,7 +4129,7 @@
       <c r="M21" s="40"/>
       <c r="N21" s="20"/>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <v>20</v>
       </c>
@@ -4549,7 +4548,7 @@
       </c>
       <c r="N31" s="20"/>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <v>30</v>
       </c>
@@ -4585,7 +4584,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="20"/>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="29">
         <v>31</v>
       </c>
@@ -4627,7 +4626,7 @@
       </c>
       <c r="N33" s="20"/>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="29">
         <v>32</v>
       </c>
@@ -4663,7 +4662,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="20"/>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="29">
         <v>33</v>
       </c>
@@ -4705,7 +4704,7 @@
       </c>
       <c r="N35" s="20"/>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <v>34</v>
       </c>
@@ -4741,7 +4740,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="20"/>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="29">
         <v>35</v>
       </c>
@@ -4783,7 +4782,7 @@
       </c>
       <c r="N37" s="20"/>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="29">
         <v>36</v>
       </c>
@@ -4861,7 +4860,7 @@
       </c>
       <c r="N39" s="20"/>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
         <v>38</v>
       </c>
@@ -4903,7 +4902,7 @@
       </c>
       <c r="N40" s="20"/>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="29">
         <v>39</v>
       </c>
@@ -4945,7 +4944,7 @@
       </c>
       <c r="N41" s="20"/>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="29">
         <v>40</v>
       </c>
@@ -5072,7 +5071,7 @@
       </c>
       <c r="N44" s="20"/>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="29">
         <v>43</v>
       </c>
@@ -5114,7 +5113,7 @@
       </c>
       <c r="N45" s="20"/>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="29">
         <v>44</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="29">
         <v>45</v>
       </c>
@@ -5201,7 +5200,7 @@
       </c>
       <c r="N47" s="20"/>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="29">
         <v>46</v>
       </c>
@@ -5243,7 +5242,7 @@
       </c>
       <c r="N48" s="20"/>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="29">
         <v>47</v>
       </c>
@@ -5530,7 +5529,7 @@
       </c>
       <c r="N55" s="20"/>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="29">
         <v>54</v>
       </c>
@@ -5572,7 +5571,7 @@
       </c>
       <c r="N56" s="20"/>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="29">
         <v>55</v>
       </c>
@@ -5614,7 +5613,7 @@
       </c>
       <c r="N57" s="20"/>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="29">
         <v>56</v>
       </c>
@@ -5656,7 +5655,7 @@
       </c>
       <c r="N58" s="20"/>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="29">
         <v>57</v>
       </c>
@@ -5698,7 +5697,7 @@
       </c>
       <c r="N59" s="20"/>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="29">
         <v>58</v>
       </c>
@@ -5740,7 +5739,7 @@
       </c>
       <c r="N60" s="20"/>
     </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="29">
         <v>59</v>
       </c>
@@ -5782,7 +5781,7 @@
       </c>
       <c r="N61" s="20"/>
     </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="29">
         <v>60</v>
       </c>
@@ -5824,7 +5823,7 @@
       </c>
       <c r="N62" s="20"/>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="29">
         <v>61</v>
       </c>
@@ -5866,7 +5865,7 @@
       </c>
       <c r="N63" s="20"/>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="29">
         <v>62</v>
       </c>
@@ -5908,7 +5907,7 @@
       </c>
       <c r="N64" s="20"/>
     </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="29">
         <v>63</v>
       </c>
@@ -5944,7 +5943,7 @@
       <c r="M65" s="6"/>
       <c r="N65" s="20"/>
     </row>
-    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="29">
         <v>64</v>
       </c>
@@ -5986,7 +5985,7 @@
       </c>
       <c r="N66" s="20"/>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="29">
         <v>65</v>
       </c>
@@ -6028,7 +6027,7 @@
       </c>
       <c r="N67" s="20"/>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="29">
         <v>66</v>
       </c>
@@ -6070,7 +6069,7 @@
       </c>
       <c r="N68" s="20"/>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="29">
         <v>67</v>
       </c>
@@ -6112,7 +6111,7 @@
       </c>
       <c r="N69" s="20"/>
     </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="29">
         <v>68</v>
       </c>
@@ -6154,7 +6153,7 @@
       </c>
       <c r="N70" s="20"/>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="29">
         <v>69</v>
       </c>
@@ -6196,7 +6195,7 @@
       </c>
       <c r="N71" s="20"/>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="29">
         <v>70</v>
       </c>
@@ -6238,7 +6237,7 @@
       </c>
       <c r="N72" s="20"/>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="29">
         <v>71</v>
       </c>
@@ -6280,7 +6279,7 @@
       </c>
       <c r="N73" s="20"/>
     </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="29">
         <v>72</v>
       </c>
@@ -6322,7 +6321,7 @@
       </c>
       <c r="N74" s="20"/>
     </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="29">
         <v>73</v>
       </c>
@@ -6358,7 +6357,7 @@
       <c r="M75" s="6"/>
       <c r="N75" s="20"/>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="29">
         <v>74</v>
       </c>
@@ -6400,7 +6399,7 @@
       </c>
       <c r="N76" s="20"/>
     </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="29">
         <v>75</v>
       </c>
@@ -6444,7 +6443,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="29">
         <v>76</v>
       </c>
@@ -6486,7 +6485,7 @@
       </c>
       <c r="N78" s="20"/>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="29">
         <v>77</v>
       </c>
@@ -6528,7 +6527,7 @@
       </c>
       <c r="N79" s="20"/>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="29">
         <v>78</v>
       </c>
@@ -6570,7 +6569,7 @@
       </c>
       <c r="N80" s="20"/>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="29">
         <v>79</v>
       </c>
@@ -6614,7 +6613,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="29">
         <v>80</v>
       </c>
@@ -6654,7 +6653,7 @@
       </c>
       <c r="N82" s="20"/>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="29">
         <v>81</v>
       </c>
@@ -6694,7 +6693,7 @@
       </c>
       <c r="N83" s="20"/>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="29">
         <v>82</v>
       </c>
@@ -6738,7 +6737,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="29"/>
       <c r="B85" s="29" t="s">
         <v>174</v>
@@ -6909,7 +6908,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="29">
         <v>86</v>
       </c>
@@ -6991,7 +6990,7 @@
       </c>
       <c r="N90" s="20"/>
     </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="29">
         <v>88</v>
       </c>
@@ -7033,7 +7032,7 @@
       </c>
       <c r="N91" s="20"/>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="29">
         <v>89</v>
       </c>
@@ -7077,7 +7076,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="29">
         <v>90</v>
       </c>
@@ -7119,7 +7118,7 @@
       </c>
       <c r="N93" s="20"/>
     </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="29">
         <v>91</v>
       </c>
@@ -7289,7 +7288,7 @@
       </c>
       <c r="N97" s="20"/>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="29">
         <v>95</v>
       </c>
@@ -7329,7 +7328,7 @@
       </c>
       <c r="N98" s="20"/>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="29">
         <v>96</v>
       </c>
@@ -7371,7 +7370,7 @@
       </c>
       <c r="N99" s="20"/>
     </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="29">
         <v>97</v>
       </c>
@@ -7411,7 +7410,7 @@
       </c>
       <c r="N100" s="20"/>
     </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="29">
         <v>98</v>
       </c>
@@ -7453,7 +7452,7 @@
       </c>
       <c r="N101" s="20"/>
     </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="29">
         <v>99</v>
       </c>
@@ -7493,7 +7492,7 @@
       </c>
       <c r="N102" s="20"/>
     </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="29">
         <v>100</v>
       </c>
@@ -7535,7 +7534,7 @@
       </c>
       <c r="N103" s="20"/>
     </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="29">
         <v>101</v>
       </c>
@@ -8419,7 +8418,7 @@
       <c r="M125" s="14"/>
       <c r="N125" s="20"/>
     </row>
-    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="29">
         <v>123</v>
       </c>
@@ -8459,7 +8458,7 @@
       </c>
       <c r="N126" s="20"/>
     </row>
-    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="29">
         <v>124</v>
       </c>
@@ -8499,7 +8498,7 @@
       </c>
       <c r="N127" s="20"/>
     </row>
-    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="29">
         <v>125</v>
       </c>
@@ -8539,7 +8538,7 @@
       </c>
       <c r="N128" s="20"/>
     </row>
-    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="29">
         <v>126</v>
       </c>
@@ -9769,11 +9768,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G59">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="endsWith" dxfId="17" priority="2" operator="endsWith" text="vacant}">
+      <formula>RIGHT(G59,LEN("vacant}"))="vacant}"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G59)),NOT(ISNUMBER(SEARCH("-&gt;",G59))))</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="16" priority="2" operator="endsWith" text="vacant}">
-      <formula>RIGHT(G59,LEN("vacant}"))="vacant}"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="15" priority="3">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G59)),(ISNUMBER(SEARCH("-&gt;",G59))))</formula>

</xml_diff>